<commit_message>
update readme and record
</commit_message>
<xml_diff>
--- a/misc/record/Time and Payment.xlsx
+++ b/misc/record/Time and Payment.xlsx
@@ -1,39 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/GitHub/Fortune500_SDG_Analysis/record/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0A3D46-3AF1-E743-8042-1F96286ADAEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <bookViews>
-    <workbookView xWindow="1000" yWindow="700" windowWidth="26040" windowHeight="16860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -77,20 +55,19 @@
     <t>10.83 hour</t>
   </si>
   <si>
-    <t>8.35 hour</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
       <t>16245</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FF000000"/>
+        <color indexed="8"/>
         <rFont val="PMingLiU"/>
-        <family val="1"/>
-        <charset val="136"/>
       </rPr>
       <t>元</t>
     </r>
@@ -99,39 +76,43 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Arial"/>
-        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> (paid)</t>
     </r>
-    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>8.35 hour</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
       <t>12525</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FF000000"/>
+        <color indexed="8"/>
         <rFont val="PMingLiU"/>
-        <family val="1"/>
-        <charset val="136"/>
       </rPr>
       <t>元</t>
     </r>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="176" formatCode="[h]&quot;h&quot;\ m&quot;m&quot;"/>
-    <numFmt numFmtId="177" formatCode="[m]&quot;m&quot;"/>
-    <numFmt numFmtId="178" formatCode="[h]&quot;h&quot;"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="59" formatCode="[h]&quot;h&quot; m&quot;m&quot;"/>
+    <numFmt numFmtId="60" formatCode="[m]&quot;m&quot;"/>
+    <numFmt numFmtId="61" formatCode="[h]&quot;h&quot;"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -140,28 +121,22 @@
     <font>
       <sz val="12"/>
       <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
       <name val="PMingLiU"/>
-      <family val="1"/>
-      <charset val="136"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Wawati TC"/>
-      <family val="3"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="PMingLiU"/>
-      <family val="1"/>
-      <charset val="136"/>
     </font>
   </fonts>
   <fills count="3">
@@ -203,21 +178,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="10"/>
       </left>
       <right style="thin">
@@ -226,123 +186,119 @@
       <top style="thin">
         <color indexed="10"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="46" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+  <cellXfs count="20">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="60" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="61" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="46" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="60" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFAAAAAA"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="ff00ff00"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffff00"/>
+      <rgbColor rgb="ffff00ff"/>
+      <rgbColor rgb="ff00ffff"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -544,7 +500,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -562,7 +518,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -591,7 +547,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -616,7 +572,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -641,7 +597,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -666,7 +622,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -691,7 +647,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -716,7 +672,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -741,7 +697,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -766,7 +722,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -791,7 +747,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -804,15 +760,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -829,7 +779,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -847,7 +797,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -872,7 +822,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -897,7 +847,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -922,7 +872,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -947,7 +897,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -972,7 +922,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -997,7 +947,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1022,7 +972,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1047,7 +997,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1072,7 +1022,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1085,15 +1035,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1107,7 +1051,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1125,7 +1069,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1154,7 +1098,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1179,7 +1123,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1204,7 +1148,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1229,7 +1173,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1254,7 +1198,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1279,7 +1223,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1304,7 +1248,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1329,7 +1273,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1354,7 +1298,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1367,1013 +1311,1002 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A56" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="12.6640625" style="1"/>
+    <col min="1" max="5" width="12.6719" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="12.6719" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="15.75" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="4">
         <v>44811</v>
       </c>
       <c r="B2" s="5">
-        <v>3.901388888888889</v>
+        <v>4.901388888888889</v>
       </c>
       <c r="C2" s="5">
-        <v>3.9986111111111109</v>
+        <v>4.998611111111111</v>
       </c>
       <c r="D2" s="6">
-        <f t="shared" ref="D2:D8" si="0">C2-B2</f>
-        <v>9.7222222222221877E-2</v>
+        <f>C2-B2</f>
+        <v>0.09722222222222222</v>
       </c>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" t="s" s="2">
         <v>4</v>
       </c>
       <c r="B3" s="5">
-        <v>3.8347222222222221</v>
+        <v>4.834722222222222</v>
       </c>
       <c r="C3" s="5">
-        <v>3.869444444444444</v>
+        <v>4.869444444444444</v>
       </c>
       <c r="D3" s="7">
-        <f t="shared" si="0"/>
-        <v>3.4722222222221877E-2</v>
+        <f>C3-B3</f>
+        <v>0.03472222222222222</v>
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="4">
         <v>44815</v>
       </c>
       <c r="B4" s="5">
-        <v>3.645833333333333</v>
+        <v>4.645833333333333</v>
       </c>
       <c r="C4" s="5">
-        <v>3.6944444444444451</v>
+        <v>4.694444444444445</v>
       </c>
       <c r="D4" s="6">
-        <f t="shared" si="0"/>
-        <v>4.8611111111112049E-2</v>
+        <f>C4-B4</f>
+        <v>0.04861111111111111</v>
       </c>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="4">
         <v>44821</v>
       </c>
       <c r="B5" s="5">
-        <v>3.875</v>
+        <v>4.875</v>
       </c>
       <c r="C5" s="5">
-        <v>3.941666666666666</v>
+        <v>4.941666666666666</v>
       </c>
       <c r="D5" s="6">
-        <f t="shared" si="0"/>
-        <v>6.6666666666665986E-2</v>
+        <f>C5-B5</f>
+        <v>0.06666666666666667</v>
       </c>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="4">
         <v>44824</v>
       </c>
       <c r="B6" s="5">
-        <v>3.9375</v>
+        <v>4.9375</v>
       </c>
       <c r="C6" s="5">
-        <v>3.979166666666667</v>
+        <v>4.979166666666667</v>
       </c>
       <c r="D6" s="8">
-        <f t="shared" si="0"/>
-        <v>4.1666666666666963E-2</v>
+        <f>C6-B6</f>
+        <v>0.04166666666666666</v>
       </c>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="4">
         <v>44828</v>
       </c>
       <c r="B7" s="5">
-        <v>3.9444444444444451</v>
+        <v>4.944444444444445</v>
       </c>
       <c r="C7" s="5">
-        <v>3.9861111111111112</v>
+        <v>4.986111111111111</v>
       </c>
       <c r="D7" s="8">
-        <f t="shared" si="0"/>
-        <v>4.1666666666666075E-2</v>
+        <f>C7-B7</f>
+        <v>0.04166666666666666</v>
       </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="4">
         <v>44829</v>
       </c>
       <c r="B8" s="5">
-        <v>3.708333333333333</v>
+        <v>4.708333333333333</v>
       </c>
       <c r="C8" s="5">
-        <v>3.8062499999999999</v>
+        <v>4.80625</v>
       </c>
       <c r="D8" s="6">
-        <f t="shared" si="0"/>
-        <v>9.7916666666666874E-2</v>
+        <f>C8-B8</f>
+        <v>0.09791666666666667</v>
       </c>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="2" t="s">
+      <c r="D9" t="s" s="2">
         <v>5</v>
       </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="4">
         <v>44836</v>
       </c>
       <c r="B10" s="5">
-        <v>3.416666666666667</v>
+        <v>4.416666666666667</v>
       </c>
       <c r="C10" s="5">
-        <v>3.5708333333333329</v>
+        <v>4.570833333333333</v>
       </c>
       <c r="D10" s="6">
-        <f t="shared" ref="D10:D18" si="1">C10-B10</f>
-        <v>0.1541666666666659</v>
+        <f>C10-B10</f>
+        <v>0.1541666666666667</v>
       </c>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="4">
         <v>44836</v>
       </c>
       <c r="B11" s="5">
-        <v>3.708333333333333</v>
+        <v>4.708333333333333</v>
       </c>
       <c r="C11" s="5">
-        <v>3.7777777777777781</v>
+        <v>4.777777777777778</v>
       </c>
       <c r="D11" s="6">
-        <f t="shared" si="1"/>
-        <v>6.9444444444445086E-2</v>
+        <f>C11-B11</f>
+        <v>0.06944444444444445</v>
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="4">
         <v>44842</v>
       </c>
       <c r="B12" s="5">
-        <v>3.833333333333333</v>
+        <v>4.833333333333333</v>
       </c>
       <c r="C12" s="5">
-        <v>3.895833333333333</v>
+        <v>4.895833333333333</v>
       </c>
       <c r="D12" s="6">
-        <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <f>C12-B12</f>
+        <v>0.0625</v>
       </c>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="4">
         <v>44843</v>
       </c>
       <c r="B13" s="5">
-        <v>3.708333333333333</v>
+        <v>4.708333333333333</v>
       </c>
       <c r="C13" s="5">
-        <v>3.7743055555555549</v>
+        <v>4.774305555555555</v>
       </c>
       <c r="D13" s="6">
-        <f t="shared" si="1"/>
-        <v>6.5972222222221877E-2</v>
+        <f>C13-B13</f>
+        <v>0.06597222222222222</v>
       </c>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="4">
         <v>44856</v>
       </c>
       <c r="B14" s="5">
-        <v>3.933333333333334</v>
+        <v>4.933333333333334</v>
       </c>
       <c r="C14" s="5">
-        <v>3.9715277777777782</v>
+        <v>4.971527777777778</v>
       </c>
       <c r="D14" s="7">
-        <f t="shared" si="1"/>
-        <v>3.8194444444444198E-2</v>
+        <f>C14-B14</f>
+        <v>0.03819444444444445</v>
       </c>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="4">
         <v>44857</v>
       </c>
       <c r="B15" s="5">
-        <v>3.708333333333333</v>
+        <v>4.708333333333333</v>
       </c>
       <c r="C15" s="5">
-        <v>3.7833333333333332</v>
+        <v>4.783333333333333</v>
       </c>
       <c r="D15" s="6">
-        <f t="shared" si="1"/>
-        <v>7.5000000000000178E-2</v>
+        <f>C15-B15</f>
+        <v>0.075</v>
       </c>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="4">
         <v>44863</v>
       </c>
       <c r="B16" s="5">
-        <v>3.4493055555555561</v>
+        <v>4.449305555555555</v>
       </c>
       <c r="C16" s="5">
-        <v>3.4930555555555549</v>
+        <v>4.493055555555555</v>
       </c>
       <c r="D16" s="6">
-        <f t="shared" si="1"/>
-        <v>4.3749999999998845E-2</v>
+        <f>C16-B16</f>
+        <v>0.04375</v>
       </c>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="4">
         <v>44863</v>
       </c>
       <c r="B17" s="5">
-        <v>3.665972222222222</v>
+        <v>4.665972222222222</v>
       </c>
       <c r="C17" s="5">
-        <v>3.7173611111111109</v>
+        <v>4.717361111111111</v>
       </c>
       <c r="D17" s="6">
-        <f t="shared" si="1"/>
-        <v>5.1388888888888928E-2</v>
+        <f>C17-B17</f>
+        <v>0.05138888888888889</v>
       </c>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="4">
         <v>44863</v>
       </c>
       <c r="B18" s="5">
-        <v>3.722916666666666</v>
+        <v>4.722916666666666</v>
       </c>
       <c r="C18" s="5">
-        <v>3.8041666666666671</v>
+        <v>4.804166666666667</v>
       </c>
       <c r="D18" s="6">
-        <f t="shared" si="1"/>
-        <v>8.1250000000001155E-2</v>
+        <f>C18-B18</f>
+        <v>0.08125</v>
       </c>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="9" t="s">
+      <c r="D19" t="s" s="9">
         <v>6</v>
       </c>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="4">
         <v>44868</v>
       </c>
       <c r="B20" s="5">
-        <v>3.943055555555556</v>
+        <v>4.943055555555556</v>
       </c>
       <c r="C20" s="5">
-        <v>3.990277777777778</v>
+        <v>4.990277777777778</v>
       </c>
       <c r="D20" s="6">
         <f>C20-B20</f>
-        <v>4.7222222222222054E-2</v>
+        <v>0.04722222222222222</v>
       </c>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="4">
         <v>44869</v>
       </c>
       <c r="B21" s="5">
-        <v>3.3597222222222221</v>
+        <v>4.359722222222222</v>
       </c>
       <c r="C21" s="5">
-        <v>3.401388888888889</v>
+        <v>4.401388888888889</v>
       </c>
       <c r="D21" s="8">
         <f>C21-B21</f>
-        <v>4.1666666666666963E-2</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="4">
         <v>44870</v>
       </c>
       <c r="B22" s="5">
-        <v>3.916666666666667</v>
+        <v>4.916666666666667</v>
       </c>
       <c r="C22" s="10">
         <v>1.002777777777778</v>
       </c>
       <c r="D22" s="5">
         <f>C22-B22</f>
-        <v>-2.9138888888888888</v>
       </c>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="4">
         <v>44871</v>
       </c>
       <c r="B23" s="5">
-        <v>3.7152777777777781</v>
+        <v>4.715277777777778</v>
       </c>
       <c r="C23" s="10">
         <v>0.8041666666666667</v>
       </c>
       <c r="D23" s="5">
         <f>C23*24-B23</f>
-        <v>15.584722222222222</v>
       </c>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="4">
         <v>44977</v>
       </c>
       <c r="B24" s="5">
-        <v>3.75</v>
+        <v>4.75</v>
       </c>
       <c r="C24" s="5">
-        <v>3.8208333333333329</v>
+        <v>4.820833333333333</v>
       </c>
       <c r="D24" s="6">
         <f>C24-B24</f>
-        <v>7.083333333333286E-2</v>
+        <v>0.07083333333333333</v>
       </c>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="2" t="s">
+      <c r="D25" t="s" s="2">
         <v>7</v>
       </c>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="4">
         <v>44991</v>
       </c>
       <c r="B26" s="5">
-        <v>3.8888888888888888</v>
+        <v>4.888888888888889</v>
       </c>
       <c r="C26" s="5">
-        <v>3.9930555555555549</v>
+        <v>4.993055555555555</v>
       </c>
       <c r="D26" s="6">
         <f>C26-B26</f>
-        <v>0.10416666666666607</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="4">
         <v>44994</v>
       </c>
       <c r="B27" s="5">
-        <v>3.875</v>
+        <v>4.875</v>
       </c>
       <c r="C27" s="5">
-        <v>3.958333333333333</v>
+        <v>4.958333333333333</v>
       </c>
       <c r="D27" s="8">
         <f>C27-B27</f>
-        <v>8.3333333333333037E-2</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="4">
         <v>45004</v>
       </c>
       <c r="B28" s="5">
-        <v>3.75</v>
+        <v>4.75</v>
       </c>
       <c r="C28" s="5">
-        <v>3.843055555555555</v>
+        <v>4.843055555555556</v>
       </c>
       <c r="D28" s="6">
         <f>C28-B28</f>
-        <v>9.3055555555555003E-2</v>
+        <v>0.09305555555555556</v>
       </c>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="4">
         <v>45011</v>
       </c>
       <c r="B29" s="5">
-        <v>3.708333333333333</v>
+        <v>4.708333333333333</v>
       </c>
       <c r="C29" s="5">
-        <v>3.8</v>
+        <v>4.8</v>
       </c>
       <c r="D29" s="6">
         <f>C29-B29</f>
-        <v>9.1666666666666785E-2</v>
+        <v>0.09166666666666666</v>
       </c>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="4">
         <v>45018</v>
       </c>
       <c r="B30" s="5">
-        <v>3.708333333333333</v>
+        <v>4.708333333333333</v>
       </c>
       <c r="C30" s="5">
-        <v>3.8034722222222221</v>
+        <v>4.803472222222222</v>
       </c>
       <c r="D30" s="6">
         <f>C30-B30</f>
-        <v>9.5138888888889106E-2</v>
+        <v>0.09513888888888888</v>
       </c>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="6">
-        <v>0.46736111111111112</v>
-      </c>
-      <c r="E31" s="2" t="s">
+        <v>0.4673611111111111</v>
+      </c>
+      <c r="E31" t="s" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="4">
         <v>45032</v>
       </c>
       <c r="B32" s="5">
-        <v>3.708333333333333</v>
+        <v>4.708333333333333</v>
       </c>
       <c r="C32" s="5">
-        <v>3.7777777777777781</v>
+        <v>4.777777777777778</v>
       </c>
       <c r="D32" s="6">
-        <f t="shared" ref="D32:D38" si="2">C32-B32</f>
-        <v>6.9444444444445086E-2</v>
+        <f>C32-B32</f>
+        <v>0.06944444444444445</v>
       </c>
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="4">
         <v>45039</v>
       </c>
       <c r="B33" s="5">
-        <v>3.708333333333333</v>
+        <v>4.708333333333333</v>
       </c>
       <c r="C33" s="5">
-        <v>3.802083333333333</v>
+        <v>4.802083333333333</v>
       </c>
       <c r="D33" s="6">
-        <f t="shared" si="2"/>
-        <v>9.375E-2</v>
+        <f>C33-B33</f>
+        <v>0.09375</v>
       </c>
       <c r="E33" s="3"/>
     </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="4">
         <v>45046</v>
       </c>
       <c r="B34" s="5">
-        <v>3.7152777777777781</v>
+        <v>4.715277777777778</v>
       </c>
       <c r="C34" s="5">
-        <v>3.8152777777777782</v>
+        <v>4.815277777777778</v>
       </c>
       <c r="D34" s="6">
-        <f t="shared" si="2"/>
-        <v>0.10000000000000009</v>
+        <f>C34-B34</f>
+        <v>0.1</v>
       </c>
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="4">
         <v>45060</v>
       </c>
       <c r="B35" s="5">
-        <v>3.708333333333333</v>
+        <v>4.708333333333333</v>
       </c>
       <c r="C35" s="5">
-        <v>3.8111111111111109</v>
+        <v>4.811111111111111</v>
       </c>
       <c r="D35" s="6">
-        <f t="shared" si="2"/>
-        <v>0.10277777777777786</v>
+        <f>C35-B35</f>
+        <v>0.1027777777777778</v>
       </c>
       <c r="E35" s="3"/>
     </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="4">
         <v>45067</v>
       </c>
       <c r="B36" s="5">
-        <v>3.71875</v>
+        <v>4.71875</v>
       </c>
       <c r="C36" s="5">
-        <v>3.791666666666667</v>
+        <v>4.791666666666667</v>
       </c>
       <c r="D36" s="6">
-        <f t="shared" si="2"/>
-        <v>7.2916666666666963E-2</v>
+        <f>C36-B36</f>
+        <v>0.07291666666666667</v>
       </c>
       <c r="E36" s="3"/>
     </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="4">
         <v>45084</v>
       </c>
       <c r="B37" s="5">
-        <v>3.7520833333333332</v>
+        <v>4.752083333333333</v>
       </c>
       <c r="C37" s="5">
-        <v>3.807638888888889</v>
+        <v>4.807638888888889</v>
       </c>
       <c r="D37" s="6">
-        <f t="shared" si="2"/>
-        <v>5.5555555555555802E-2</v>
+        <f>C37-B37</f>
+        <v>0.05555555555555555</v>
       </c>
       <c r="E37" s="3"/>
     </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="11">
         <v>45096</v>
       </c>
       <c r="B38" s="5">
-        <v>3.7152777777777781</v>
+        <v>4.715277777777778</v>
       </c>
       <c r="C38" s="5">
-        <v>3.786111111111111</v>
+        <v>4.786111111111111</v>
       </c>
       <c r="D38" s="6">
-        <f t="shared" si="2"/>
-        <v>7.083333333333286E-2</v>
+        <f>C38-B38</f>
+        <v>0.07083333333333333</v>
       </c>
       <c r="E38" s="3"/>
     </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
-      <c r="D39" s="2" t="s">
+      <c r="D39" t="s" s="2">
         <v>9</v>
       </c>
       <c r="E39" s="3"/>
     </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="4">
         <v>45100</v>
       </c>
       <c r="B40" s="5">
-        <v>3.0402777777777779</v>
+        <v>4.040277777777778</v>
       </c>
       <c r="C40" s="5">
-        <v>3.0798611111111112</v>
+        <v>4.079861111111111</v>
       </c>
       <c r="D40" s="7">
-        <f t="shared" ref="D40:D45" si="3">C40-B40</f>
-        <v>3.9583333333333304E-2</v>
+        <f>C40-B40</f>
+        <v>0.03958333333333333</v>
       </c>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="4">
         <v>45108</v>
       </c>
       <c r="B41" s="5">
-        <v>3.708333333333333</v>
+        <v>4.708333333333333</v>
       </c>
       <c r="C41" s="5">
-        <v>3.8402777777777781</v>
+        <v>4.840277777777778</v>
       </c>
       <c r="D41" s="6">
-        <f t="shared" si="3"/>
-        <v>0.13194444444444509</v>
+        <f>C41-B41</f>
+        <v>0.1319444444444444</v>
       </c>
       <c r="E41" s="3"/>
     </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="4">
         <v>45116</v>
       </c>
       <c r="B42" s="5">
-        <v>3.729166666666667</v>
+        <v>4.729166666666667</v>
       </c>
       <c r="C42" s="5">
-        <v>3.8125</v>
+        <v>4.8125</v>
       </c>
       <c r="D42" s="8">
-        <f t="shared" si="3"/>
-        <v>8.3333333333333037E-2</v>
+        <f>C42-B42</f>
+        <v>0.08333333333333333</v>
       </c>
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="4">
         <v>45138</v>
       </c>
       <c r="B43" s="5">
-        <v>3.729166666666667</v>
+        <v>4.729166666666667</v>
       </c>
       <c r="C43" s="5">
-        <v>3.8298611111111112</v>
+        <v>4.829861111111111</v>
       </c>
       <c r="D43" s="6">
-        <f t="shared" si="3"/>
-        <v>0.1006944444444442</v>
+        <f>C43-B43</f>
+        <v>0.1006944444444444</v>
       </c>
       <c r="E43" s="3"/>
     </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="4">
         <v>45158</v>
       </c>
       <c r="B44" s="5">
-        <v>3.71875</v>
+        <v>4.71875</v>
       </c>
       <c r="C44" s="5">
-        <v>3.7951388888888888</v>
+        <v>4.795138888888889</v>
       </c>
       <c r="D44" s="6">
-        <f t="shared" si="3"/>
-        <v>7.638888888888884E-2</v>
+        <f>C44-B44</f>
+        <v>0.0763888888888889</v>
       </c>
       <c r="E44" s="3"/>
     </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="4">
         <v>45165</v>
       </c>
       <c r="B45" s="5">
-        <v>3.708333333333333</v>
+        <v>4.708333333333333</v>
       </c>
       <c r="C45" s="5">
-        <v>3.7743055555555549</v>
+        <v>4.774305555555555</v>
       </c>
       <c r="D45" s="6">
-        <f t="shared" si="3"/>
-        <v>6.5972222222221877E-2</v>
+        <f>C45-B45</f>
+        <v>0.06597222222222222</v>
       </c>
       <c r="E45" s="3"/>
     </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="6">
-        <v>0.49791666666666667</v>
-      </c>
-      <c r="E46" s="2" t="s">
+        <v>0.4979166666666667</v>
+      </c>
+      <c r="E46" t="s" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="4">
         <v>45179</v>
       </c>
       <c r="B47" s="5">
-        <v>3.729166666666667</v>
+        <v>4.729166666666667</v>
       </c>
       <c r="C47" s="5">
-        <v>3.802083333333333</v>
+        <v>4.802083333333333</v>
       </c>
       <c r="D47" s="6">
-        <f t="shared" ref="D47:D54" si="4">C47-B47</f>
-        <v>7.2916666666666075E-2</v>
+        <f>C47-B47</f>
+        <v>0.07291666666666667</v>
       </c>
       <c r="E47" s="3"/>
     </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="4">
         <v>45186</v>
       </c>
       <c r="B48" s="5">
-        <v>3.708333333333333</v>
+        <v>4.708333333333333</v>
       </c>
       <c r="C48" s="5">
-        <v>3.7986111111111112</v>
+        <v>4.798611111111111</v>
       </c>
       <c r="D48" s="6">
-        <f t="shared" si="4"/>
-        <v>9.0277777777778123E-2</v>
+        <f>C48-B48</f>
+        <v>0.09027777777777778</v>
       </c>
       <c r="E48" s="3"/>
     </row>
-    <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="4">
         <v>45193</v>
       </c>
       <c r="B49" s="5">
-        <v>3.7152777777777781</v>
+        <v>4.715277777777778</v>
       </c>
       <c r="C49" s="5">
-        <v>3.807638888888889</v>
+        <v>4.807638888888889</v>
       </c>
       <c r="D49" s="6">
-        <f t="shared" si="4"/>
-        <v>9.2361111111110894E-2</v>
+        <f>C49-B49</f>
+        <v>0.09236111111111112</v>
       </c>
       <c r="E49" s="3"/>
     </row>
-    <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="4">
         <v>45200</v>
       </c>
       <c r="B50" s="5">
-        <v>3.71875</v>
+        <v>4.71875</v>
       </c>
       <c r="C50" s="5">
-        <v>3.8090277777777781</v>
+        <v>4.809027777777778</v>
       </c>
       <c r="D50" s="6">
-        <f t="shared" si="4"/>
-        <v>9.0277777777778123E-2</v>
+        <f>C50-B50</f>
+        <v>0.09027777777777778</v>
       </c>
       <c r="E50" s="3"/>
     </row>
-    <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="4">
         <v>45222</v>
       </c>
       <c r="B51" s="5">
-        <v>3.833333333333333</v>
+        <v>4.833333333333333</v>
       </c>
       <c r="C51" s="5">
-        <v>3.936805555555555</v>
+        <v>4.936805555555556</v>
       </c>
       <c r="D51" s="6">
-        <f t="shared" si="4"/>
-        <v>0.10347222222222197</v>
+        <f>C51-B51</f>
+        <v>0.1034722222222222</v>
       </c>
       <c r="E51" s="3"/>
     </row>
-    <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="4">
         <v>45224</v>
       </c>
       <c r="B52" s="5">
-        <v>3.875</v>
+        <v>4.875</v>
       </c>
       <c r="C52" s="5">
-        <v>3.916666666666667</v>
+        <v>4.916666666666667</v>
       </c>
       <c r="D52" s="8">
-        <f t="shared" si="4"/>
-        <v>4.1666666666666963E-2</v>
+        <f>C52-B52</f>
+        <v>0.04166666666666666</v>
       </c>
       <c r="E52" s="3"/>
     </row>
-    <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="4">
         <v>45241</v>
       </c>
       <c r="B53" s="5">
-        <v>3.8715277777777781</v>
+        <v>4.871527777777778</v>
       </c>
       <c r="C53" s="5">
-        <v>3.916666666666667</v>
+        <v>4.916666666666667</v>
       </c>
       <c r="D53" s="6">
-        <f t="shared" si="4"/>
-        <v>4.513888888888884E-2</v>
+        <f>C53-B53</f>
+        <v>0.04513888888888889</v>
       </c>
       <c r="E53" s="3"/>
     </row>
-    <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="4">
         <v>45242</v>
       </c>
       <c r="B54" s="5">
-        <v>3.708333333333333</v>
+        <v>4.708333333333333</v>
       </c>
       <c r="C54" s="5">
-        <v>3.791666666666667</v>
+        <v>4.791666666666667</v>
       </c>
       <c r="D54" s="8">
-        <f t="shared" si="4"/>
-        <v>8.3333333333333925E-2</v>
+        <f>C54-B54</f>
+        <v>0.08333333333333333</v>
       </c>
       <c r="E54" s="3"/>
     </row>
-    <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
-      <c r="D55" s="2" t="s">
+      <c r="D55" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="E55" t="s" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="4">
         <v>45263</v>
       </c>
       <c r="B56" s="5">
-        <v>3.708333333333333</v>
+        <v>4.708333333333333</v>
       </c>
       <c r="C56" s="5">
-        <v>3.802083333333333</v>
+        <v>4.802083333333333</v>
       </c>
       <c r="D56" s="6">
         <f>C56-B56</f>
-        <v>9.375E-2</v>
+        <v>0.09375</v>
       </c>
       <c r="E56" s="3"/>
     </row>
-    <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="4">
         <v>45275</v>
       </c>
       <c r="B57" s="5">
-        <v>3.75</v>
+        <v>4.75</v>
       </c>
       <c r="C57" s="5">
-        <v>3.8472222222222219</v>
+        <v>4.847222222222222</v>
       </c>
       <c r="D57" s="6">
         <f>C57-B57</f>
-        <v>9.7222222222221877E-2</v>
+        <v>0.09722222222222222</v>
       </c>
       <c r="E57" s="3"/>
     </row>
-    <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="4">
         <v>45305</v>
       </c>
       <c r="B58" s="5">
-        <v>3.708333333333333</v>
+        <v>4.708333333333333</v>
       </c>
       <c r="C58" s="5">
-        <v>3.7673611111111112</v>
+        <v>4.767361111111111</v>
       </c>
       <c r="D58" s="6">
         <f>C58-B58</f>
-        <v>5.9027777777778123E-2</v>
+        <v>0.05902777777777778</v>
       </c>
       <c r="E58" s="3"/>
     </row>
-    <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="4">
         <v>45312</v>
       </c>
       <c r="B59" s="5">
-        <v>3.354166666666667</v>
+        <v>4.354166666666667</v>
       </c>
       <c r="C59" s="5">
-        <v>3.395833333333333</v>
+        <v>4.395833333333333</v>
       </c>
       <c r="D59" s="8">
         <f>C59-B59</f>
-        <v>4.1666666666666075E-2</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="E59" s="3"/>
     </row>
-    <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="4">
         <v>45312</v>
       </c>
       <c r="B60" s="5">
-        <v>3.666666666666667</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="C60" s="5">
-        <v>3.7430555555555549</v>
+        <v>4.743055555555555</v>
       </c>
       <c r="D60" s="6">
         <f>C60-B60</f>
-        <v>7.6388888888887951E-2</v>
+        <v>0.0763888888888889</v>
       </c>
       <c r="E60" s="3"/>
     </row>
-    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
-      <c r="D61" s="2" t="s">
+      <c r="D61" t="s" s="2">
         <v>13</v>
       </c>
-      <c r="E61" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E61" t="s" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="4">
         <v>45403</v>
       </c>
       <c r="B62" s="5">
-        <v>3.708333333333333</v>
+        <v>4.708333333333333</v>
       </c>
       <c r="C62" s="5">
-        <v>3.8013888888888889</v>
+        <v>4.801388888888889</v>
       </c>
       <c r="D62" s="6">
-        <f t="shared" ref="D62:D67" si="5">C62-B62</f>
-        <v>9.3055555555555891E-2</v>
+        <f>C62-B62</f>
+        <v>0.09305555555555556</v>
       </c>
       <c r="E62" s="3"/>
     </row>
-    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="4">
         <v>45410</v>
       </c>
       <c r="B63" s="5">
-        <v>3.708333333333333</v>
+        <v>4.708333333333333</v>
       </c>
       <c r="C63" s="5">
-        <v>3.802083333333333</v>
+        <v>4.802083333333333</v>
       </c>
       <c r="D63" s="6">
-        <f t="shared" si="5"/>
-        <v>9.375E-2</v>
+        <f>C63-B63</f>
+        <v>0.09375</v>
       </c>
       <c r="E63" s="3"/>
     </row>
-    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="4">
         <v>45414</v>
       </c>
       <c r="B64" s="5">
-        <v>3.71875</v>
+        <v>4.71875</v>
       </c>
       <c r="C64" s="5">
-        <v>3.739583333333333</v>
+        <v>4.739583333333333</v>
       </c>
       <c r="D64" s="7">
-        <f t="shared" si="5"/>
-        <v>2.0833333333333037E-2</v>
+        <f>C64-B64</f>
+        <v>0.02083333333333333</v>
       </c>
       <c r="E64" s="3"/>
     </row>
-    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="4">
         <v>45419</v>
       </c>
@@ -2381,15 +2314,15 @@
         <v>45419.729166666664</v>
       </c>
       <c r="C65" s="5">
-        <v>45419.768750000003</v>
+        <v>45419.76875</v>
       </c>
       <c r="D65" s="7">
-        <f t="shared" si="5"/>
-        <v>3.9583333338669036E-2</v>
+        <f>C65-B65</f>
+        <v>0.03958333333885228</v>
       </c>
       <c r="E65" s="3"/>
     </row>
-    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="4">
         <v>45421</v>
       </c>
@@ -2400,184 +2333,195 @@
         <v>45421.78125</v>
       </c>
       <c r="D66" s="7">
-        <f t="shared" si="5"/>
-        <v>6.1111111113859806E-2</v>
+        <f>C66-B66</f>
+        <v>0.06111111111111111</v>
       </c>
       <c r="E66" s="3"/>
     </row>
-    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="13">
+    <row r="67" ht="15.75" customHeight="1">
+      <c r="A67" s="12">
         <v>45424</v>
       </c>
-      <c r="B67" s="14">
+      <c r="B67" s="13">
         <v>45424.708333333336</v>
       </c>
-      <c r="C67" s="14">
+      <c r="C67" s="13">
         <v>45424.747916666667</v>
       </c>
-      <c r="D67" s="15">
-        <f t="shared" si="5"/>
-        <v>3.9583333331393078E-2</v>
-      </c>
-      <c r="E67" s="16"/>
-    </row>
-    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="17"/>
-      <c r="B68" s="17"/>
-      <c r="C68" s="17"/>
-      <c r="D68" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="E68" s="18" t="s">
+      <c r="D67" s="14">
+        <f>C67-B67</f>
+        <v>0.03958333333333333</v>
+      </c>
+      <c r="E67" s="15"/>
+    </row>
+    <row r="68" ht="15.75" customHeight="1">
+      <c r="A68" s="16"/>
+      <c r="B68" s="16"/>
+      <c r="C68" s="16"/>
+      <c r="D68" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="E68" t="s" s="17">
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A69" s="19">
+    <row r="69" ht="16" customHeight="1">
+      <c r="A69" s="18">
         <v>45463</v>
       </c>
-      <c r="B69" s="20">
-        <v>0.875</v>
-      </c>
-      <c r="C69" s="20">
-        <v>0.95694444444444438</v>
-      </c>
-      <c r="D69" s="17"/>
-      <c r="E69" s="17"/>
-    </row>
-    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="19">
+      <c r="B69" s="19">
+        <v>1.875</v>
+      </c>
+      <c r="C69" s="19">
+        <v>1.956944444444444</v>
+      </c>
+      <c r="D69" s="16"/>
+      <c r="E69" s="16"/>
+    </row>
+    <row r="70" ht="15.75" customHeight="1">
+      <c r="A70" s="18">
         <v>45468</v>
       </c>
-      <c r="B70" s="20">
-        <v>0.875</v>
-      </c>
-      <c r="C70" s="20">
-        <v>0.92222222222222217</v>
-      </c>
-      <c r="D70" s="17"/>
-      <c r="E70" s="17"/>
-    </row>
-    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="19">
+      <c r="B70" s="19">
+        <v>1.875</v>
+      </c>
+      <c r="C70" s="19">
+        <v>1.922222222222222</v>
+      </c>
+      <c r="D70" s="16"/>
+      <c r="E70" s="16"/>
+    </row>
+    <row r="71" ht="15.75" customHeight="1">
+      <c r="A71" s="18">
         <v>45490</v>
       </c>
-      <c r="B71" s="20">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="C71" s="20">
-        <v>0.84861111111111109</v>
-      </c>
-      <c r="D71" s="17"/>
-      <c r="E71" s="17"/>
-    </row>
-    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="19">
+      <c r="B71" s="19">
+        <v>1.833333333333333</v>
+      </c>
+      <c r="C71" s="19">
+        <v>1.848611111111111</v>
+      </c>
+      <c r="D71" s="16"/>
+      <c r="E71" s="16"/>
+    </row>
+    <row r="72" ht="15.75" customHeight="1">
+      <c r="A72" s="18">
         <v>45498</v>
       </c>
-      <c r="B72" s="20">
-        <v>0.85416666666666663</v>
-      </c>
-      <c r="C72" s="20">
-        <v>0.89583333333333337</v>
-      </c>
-      <c r="D72" s="17"/>
-      <c r="E72" s="17"/>
-    </row>
-    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="19">
+      <c r="B72" s="19">
+        <v>1.854166666666667</v>
+      </c>
+      <c r="C72" s="19">
+        <v>1.895833333333333</v>
+      </c>
+      <c r="D72" s="16"/>
+      <c r="E72" s="16"/>
+    </row>
+    <row r="73" ht="15.75" customHeight="1">
+      <c r="A73" s="18">
         <v>45504</v>
       </c>
-      <c r="B73" s="20">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="C73" s="21">
-        <v>0.90763888888888899</v>
-      </c>
-      <c r="D73" s="17"/>
-      <c r="E73" s="17"/>
-    </row>
-    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A74" s="17"/>
-      <c r="B74" s="17"/>
-      <c r="C74" s="17"/>
-      <c r="D74" s="17"/>
-      <c r="E74" s="17"/>
-    </row>
-    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A75" s="17"/>
-      <c r="B75" s="17"/>
-      <c r="C75" s="17"/>
-      <c r="D75" s="17"/>
-      <c r="E75" s="17"/>
-    </row>
-    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="17"/>
-      <c r="B76" s="17"/>
-      <c r="C76" s="17"/>
-      <c r="D76" s="17"/>
-      <c r="E76" s="17"/>
-    </row>
-    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="17"/>
-      <c r="B77" s="17"/>
-      <c r="C77" s="17"/>
-      <c r="D77" s="17"/>
-      <c r="E77" s="17"/>
-    </row>
-    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="17"/>
-      <c r="B78" s="17"/>
-      <c r="C78" s="17"/>
-      <c r="D78" s="17"/>
-      <c r="E78" s="17"/>
-    </row>
-    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A79" s="17"/>
-      <c r="B79" s="17"/>
-      <c r="C79" s="17"/>
-      <c r="D79" s="17"/>
-      <c r="E79" s="17"/>
-    </row>
-    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A80" s="17"/>
-      <c r="B80" s="17"/>
-      <c r="C80" s="17"/>
-      <c r="D80" s="17"/>
-      <c r="E80" s="17"/>
-    </row>
-    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A81" s="17"/>
-      <c r="B81" s="17"/>
-      <c r="C81" s="17"/>
-      <c r="D81" s="17"/>
-      <c r="E81" s="17"/>
-    </row>
-    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A82" s="17"/>
-      <c r="B82" s="17"/>
-      <c r="C82" s="17"/>
-      <c r="D82" s="17"/>
-      <c r="E82" s="17"/>
-    </row>
-    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="17"/>
-      <c r="B83" s="17"/>
-      <c r="C83" s="17"/>
-      <c r="D83" s="17"/>
-      <c r="E83" s="17"/>
-    </row>
-    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A84" s="17"/>
-      <c r="B84" s="17"/>
-      <c r="C84" s="17"/>
-      <c r="D84" s="17"/>
-      <c r="E84" s="17"/>
+      <c r="B73" s="19">
+        <v>1.833333333333333</v>
+      </c>
+      <c r="C73" s="19">
+        <v>1.907638888888889</v>
+      </c>
+      <c r="D73" s="16"/>
+      <c r="E73" s="16"/>
+    </row>
+    <row r="74" ht="15.75" customHeight="1">
+      <c r="A74" s="18">
+        <v>45511</v>
+      </c>
+      <c r="B74" s="19">
+        <v>45512.627083333333</v>
+      </c>
+      <c r="C74" s="19">
+        <v>45512.68125</v>
+      </c>
+      <c r="D74" s="16"/>
+      <c r="E74" s="16"/>
+    </row>
+    <row r="75" ht="15.75" customHeight="1">
+      <c r="A75" s="18">
+        <v>45512</v>
+      </c>
+      <c r="B75" s="19">
+        <v>45512.420833333330</v>
+      </c>
+      <c r="C75" s="19">
+        <v>45512.526388888888</v>
+      </c>
+      <c r="D75" s="16"/>
+      <c r="E75" s="16"/>
+    </row>
+    <row r="76" ht="15.75" customHeight="1">
+      <c r="A76" s="16"/>
+      <c r="B76" s="16"/>
+      <c r="C76" s="16"/>
+      <c r="D76" s="16"/>
+      <c r="E76" s="16"/>
+    </row>
+    <row r="77" ht="15.75" customHeight="1">
+      <c r="A77" s="16"/>
+      <c r="B77" s="16"/>
+      <c r="C77" s="16"/>
+      <c r="D77" s="16"/>
+      <c r="E77" s="16"/>
+    </row>
+    <row r="78" ht="15.75" customHeight="1">
+      <c r="A78" s="16"/>
+      <c r="B78" s="16"/>
+      <c r="C78" s="16"/>
+      <c r="D78" s="16"/>
+      <c r="E78" s="16"/>
+    </row>
+    <row r="79" ht="15.75" customHeight="1">
+      <c r="A79" s="16"/>
+      <c r="B79" s="16"/>
+      <c r="C79" s="16"/>
+      <c r="D79" s="16"/>
+      <c r="E79" s="16"/>
+    </row>
+    <row r="80" ht="15.75" customHeight="1">
+      <c r="A80" s="16"/>
+      <c r="B80" s="16"/>
+      <c r="C80" s="16"/>
+      <c r="D80" s="16"/>
+      <c r="E80" s="16"/>
+    </row>
+    <row r="81" ht="15.75" customHeight="1">
+      <c r="A81" s="16"/>
+      <c r="B81" s="16"/>
+      <c r="C81" s="16"/>
+      <c r="D81" s="16"/>
+      <c r="E81" s="16"/>
+    </row>
+    <row r="82" ht="15.75" customHeight="1">
+      <c r="A82" s="16"/>
+      <c r="B82" s="16"/>
+      <c r="C82" s="16"/>
+      <c r="D82" s="16"/>
+      <c r="E82" s="16"/>
+    </row>
+    <row r="83" ht="15.75" customHeight="1">
+      <c r="A83" s="16"/>
+      <c r="B83" s="16"/>
+      <c r="C83" s="16"/>
+      <c r="D83" s="16"/>
+      <c r="E83" s="16"/>
+    </row>
+    <row r="84" ht="15.75" customHeight="1">
+      <c r="A84" s="16"/>
+      <c r="B84" s="16"/>
+      <c r="C84" s="16"/>
+      <c r="D84" s="16"/>
+      <c r="E84" s="16"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
lexicon and time update
</commit_message>
<xml_diff>
--- a/misc/record/Time and Payment.xlsx
+++ b/misc/record/Time and Payment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/GitHub/Fortune500_SDG_Analysis/misc/record/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26210BD8-32A2-554A-8E9D-C067DB4149E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7E7158-63A2-5541-9BEC-1E090F2E0825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-32700" yWindow="3400" windowWidth="23520" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1502,7 +1502,7 @@
   <dimension ref="A1:E103"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A73" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I98" sqref="I98"/>
+      <selection activeCell="E99" sqref="E99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2992,10 +2992,18 @@
       <c r="E98" s="24"/>
     </row>
     <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A99" s="24"/>
-      <c r="B99" s="24"/>
-      <c r="C99" s="24"/>
-      <c r="D99" s="24"/>
+      <c r="A99" s="28">
+        <v>45888</v>
+      </c>
+      <c r="B99" s="29">
+        <v>0.375</v>
+      </c>
+      <c r="C99" s="29">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D99" s="24">
+        <v>1</v>
+      </c>
       <c r="E99" s="24"/>
     </row>
     <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
update time and record
</commit_message>
<xml_diff>
--- a/misc/record/Time and Payment.xlsx
+++ b/misc/record/Time and Payment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/GitHub/Fortune500_SDG_Analysis/misc/record/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bc3139/repo/work/Fortune500_SDG_Analysis/misc/record/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B489AB57-DBD5-2D4C-8080-B90B7D5C1EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4CC9D1A-9E8F-874C-9BD3-79B98C2000CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-34740" yWindow="2120" windowWidth="28420" windowHeight="19360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -343,7 +343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -375,6 +375,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1508,7 +1509,7 @@
   <dimension ref="A1:E103"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A73" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H94" sqref="H94"/>
+      <selection activeCell="E103" sqref="E103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3041,16 +3042,28 @@
       </c>
     </row>
     <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A102" s="24"/>
-      <c r="B102" s="24"/>
-      <c r="C102" s="24"/>
-      <c r="D102" s="24"/>
+      <c r="A102" s="28">
+        <v>45895</v>
+      </c>
+      <c r="B102" s="29">
+        <v>0.5625</v>
+      </c>
+      <c r="C102" s="29">
+        <v>0.625</v>
+      </c>
+      <c r="D102" s="31"/>
       <c r="E102" s="24"/>
     </row>
     <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A103" s="24"/>
-      <c r="B103" s="24"/>
-      <c r="C103" s="24"/>
+      <c r="A103" s="28">
+        <v>45897</v>
+      </c>
+      <c r="B103" s="29">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C103" s="29">
+        <v>0.625</v>
+      </c>
       <c r="D103" s="24"/>
       <c r="E103" s="24"/>
     </row>

</xml_diff>